<commit_message>
Simplifying provision of fate
</commit_message>
<xml_diff>
--- a/forms/Form-3DC-multiple.xlsx
+++ b/forms/Form-3DC-multiple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14B7DFD-B62D-4FBE-A8EE-5E362A4D819F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8847E84-5035-4880-A0A2-0C0BFD2B5597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Cx58BKH9RAl4hR6TInwo/zSEIsJslTGCMvwi5w6Ru9YY3/pB4R7/iueTH7tzAqUuNSxg4SzE4sxcKoKKT425cg==" workbookSaltValue="L0GnnI9BWtZqZ6sYX2LnJw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
@@ -147,7 +147,7 @@
     <t>3-DC-multiple</t>
   </si>
   <si>
-    <t>Fate</t>
+    <t>Retained</t>
   </si>
 </sst>
 </file>
@@ -845,10 +845,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -957,6 +953,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1307,24 +1306,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="72"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="71"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="73"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="75"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="74"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="21"/>
@@ -1374,15 +1373,15 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="69"/>
+      <c r="D8" s="68"/>
       <c r="E8" s="13"/>
-      <c r="F8" s="69" t="s">
+      <c r="F8" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="69"/>
+      <c r="G8" s="68"/>
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1602,11 +1601,11 @@
     </row>
     <row r="30" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="10"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="68"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="67"/>
       <c r="H30" s="9"/>
     </row>
     <row r="31" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1660,15 +1659,15 @@
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" style="65" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="62" customWidth="1"/>
+    <col min="3" max="3" width="25" style="64" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="61" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" style="35" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="34" customWidth="1"/>
     <col min="7" max="7" width="12.140625" style="35" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" style="40" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="41" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" style="37" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="82" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="81" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="40"/>
     <col min="13" max="209" width="9.140625" style="41"/>
     <col min="210" max="210" width="9.140625" style="43"/>
@@ -1886,18 +1885,18 @@
       <c r="HB1"/>
     </row>
     <row r="2" spans="2:210" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="79"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="78"/>
       <c r="L2" s="27"/>
       <c r="M2" s="27"/>
       <c r="N2" s="27"/>
@@ -2099,234 +2098,234 @@
       <c r="HB2" s="28"/>
     </row>
     <row r="3" spans="2:210" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="83"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="76" t="s">
+      <c r="B3" s="82"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="77"/>
-      <c r="S3" s="77"/>
-      <c r="T3" s="77"/>
-      <c r="U3" s="77"/>
-      <c r="V3" s="77"/>
-      <c r="W3" s="77"/>
-      <c r="X3" s="77"/>
-      <c r="Y3" s="77"/>
-      <c r="Z3" s="77"/>
-      <c r="AA3" s="77"/>
-      <c r="AB3" s="77"/>
-      <c r="AC3" s="77"/>
-      <c r="AD3" s="77"/>
-      <c r="AE3" s="77"/>
-      <c r="AF3" s="77"/>
-      <c r="AG3" s="77"/>
-      <c r="AH3" s="77"/>
-      <c r="AI3" s="77"/>
-      <c r="AJ3" s="77"/>
-      <c r="AK3" s="77"/>
-      <c r="AL3" s="77"/>
-      <c r="AM3" s="77"/>
-      <c r="AN3" s="77"/>
-      <c r="AO3" s="77"/>
-      <c r="AP3" s="77"/>
-      <c r="AQ3" s="77"/>
-      <c r="AR3" s="77"/>
-      <c r="AS3" s="77"/>
-      <c r="AT3" s="77"/>
-      <c r="AU3" s="77"/>
-      <c r="AV3" s="77"/>
-      <c r="AW3" s="77"/>
-      <c r="AX3" s="77"/>
-      <c r="AY3" s="77"/>
-      <c r="AZ3" s="77"/>
-      <c r="BA3" s="77"/>
-      <c r="BB3" s="77"/>
-      <c r="BC3" s="77"/>
-      <c r="BD3" s="77"/>
-      <c r="BE3" s="77"/>
-      <c r="BF3" s="77"/>
-      <c r="BG3" s="77"/>
-      <c r="BH3" s="77"/>
-      <c r="BI3" s="77"/>
-      <c r="BJ3" s="77"/>
-      <c r="BK3" s="77"/>
-      <c r="BL3" s="77"/>
-      <c r="BM3" s="77"/>
-      <c r="BN3" s="77"/>
-      <c r="BO3" s="77"/>
-      <c r="BP3" s="77"/>
-      <c r="BQ3" s="77"/>
-      <c r="BR3" s="77"/>
-      <c r="BS3" s="77"/>
-      <c r="BT3" s="77"/>
-      <c r="BU3" s="77"/>
-      <c r="BV3" s="77"/>
-      <c r="BW3" s="77"/>
-      <c r="BX3" s="77"/>
-      <c r="BY3" s="77"/>
-      <c r="BZ3" s="77"/>
-      <c r="CA3" s="77"/>
-      <c r="CB3" s="77"/>
-      <c r="CC3" s="77"/>
-      <c r="CD3" s="77"/>
-      <c r="CE3" s="77"/>
-      <c r="CF3" s="77"/>
-      <c r="CG3" s="77"/>
-      <c r="CH3" s="77"/>
-      <c r="CI3" s="77"/>
-      <c r="CJ3" s="77"/>
-      <c r="CK3" s="77"/>
-      <c r="CL3" s="77"/>
-      <c r="CM3" s="77"/>
-      <c r="CN3" s="77"/>
-      <c r="CO3" s="77"/>
-      <c r="CP3" s="77"/>
-      <c r="CQ3" s="77"/>
-      <c r="CR3" s="77"/>
-      <c r="CS3" s="77"/>
-      <c r="CT3" s="77"/>
-      <c r="CU3" s="77"/>
-      <c r="CV3" s="77"/>
-      <c r="CW3" s="77"/>
-      <c r="CX3" s="77"/>
-      <c r="CY3" s="77"/>
-      <c r="CZ3" s="77"/>
-      <c r="DA3" s="77"/>
-      <c r="DB3" s="77"/>
-      <c r="DC3" s="77"/>
-      <c r="DD3" s="77"/>
-      <c r="DE3" s="77"/>
-      <c r="DF3" s="77"/>
-      <c r="DG3" s="77"/>
-      <c r="DH3" s="77"/>
-      <c r="DI3" s="77"/>
-      <c r="DJ3" s="77"/>
-      <c r="DK3" s="77"/>
-      <c r="DL3" s="77"/>
-      <c r="DM3" s="77"/>
-      <c r="DN3" s="77"/>
-      <c r="DO3" s="77"/>
-      <c r="DP3" s="77"/>
-      <c r="DQ3" s="77"/>
-      <c r="DR3" s="77"/>
-      <c r="DS3" s="77"/>
-      <c r="DT3" s="77"/>
-      <c r="DU3" s="77"/>
-      <c r="DV3" s="77"/>
-      <c r="DW3" s="77"/>
-      <c r="DX3" s="77"/>
-      <c r="DY3" s="77"/>
-      <c r="DZ3" s="77"/>
-      <c r="EA3" s="77"/>
-      <c r="EB3" s="77"/>
-      <c r="EC3" s="77"/>
-      <c r="ED3" s="77"/>
-      <c r="EE3" s="77"/>
-      <c r="EF3" s="77"/>
-      <c r="EG3" s="77"/>
-      <c r="EH3" s="77"/>
-      <c r="EI3" s="77"/>
-      <c r="EJ3" s="77"/>
-      <c r="EK3" s="77"/>
-      <c r="EL3" s="77"/>
-      <c r="EM3" s="77"/>
-      <c r="EN3" s="77"/>
-      <c r="EO3" s="77"/>
-      <c r="EP3" s="77"/>
-      <c r="EQ3" s="77"/>
-      <c r="ER3" s="77"/>
-      <c r="ES3" s="77"/>
-      <c r="ET3" s="77"/>
-      <c r="EU3" s="77"/>
-      <c r="EV3" s="77"/>
-      <c r="EW3" s="77"/>
-      <c r="EX3" s="77"/>
-      <c r="EY3" s="77"/>
-      <c r="EZ3" s="77"/>
-      <c r="FA3" s="77"/>
-      <c r="FB3" s="77"/>
-      <c r="FC3" s="77"/>
-      <c r="FD3" s="77"/>
-      <c r="FE3" s="77"/>
-      <c r="FF3" s="77"/>
-      <c r="FG3" s="77"/>
-      <c r="FH3" s="77"/>
-      <c r="FI3" s="77"/>
-      <c r="FJ3" s="77"/>
-      <c r="FK3" s="77"/>
-      <c r="FL3" s="77"/>
-      <c r="FM3" s="77"/>
-      <c r="FN3" s="77"/>
-      <c r="FO3" s="77"/>
-      <c r="FP3" s="77"/>
-      <c r="FQ3" s="77"/>
-      <c r="FR3" s="77"/>
-      <c r="FS3" s="77"/>
-      <c r="FT3" s="77"/>
-      <c r="FU3" s="77"/>
-      <c r="FV3" s="77"/>
-      <c r="FW3" s="77"/>
-      <c r="FX3" s="77"/>
-      <c r="FY3" s="77"/>
-      <c r="FZ3" s="77"/>
-      <c r="GA3" s="77"/>
-      <c r="GB3" s="77"/>
-      <c r="GC3" s="77"/>
-      <c r="GD3" s="77"/>
-      <c r="GE3" s="77"/>
-      <c r="GF3" s="77"/>
-      <c r="GG3" s="77"/>
-      <c r="GH3" s="77"/>
-      <c r="GI3" s="77"/>
-      <c r="GJ3" s="77"/>
-      <c r="GK3" s="77"/>
-      <c r="GL3" s="77"/>
-      <c r="GM3" s="77"/>
-      <c r="GN3" s="77"/>
-      <c r="GO3" s="77"/>
-      <c r="GP3" s="77"/>
-      <c r="GQ3" s="77"/>
-      <c r="GR3" s="77"/>
-      <c r="GS3" s="77"/>
-      <c r="GT3" s="77"/>
-      <c r="GU3" s="77"/>
-      <c r="GV3" s="77"/>
-      <c r="GW3" s="77"/>
-      <c r="GX3" s="77"/>
-      <c r="GY3" s="77"/>
-      <c r="GZ3" s="77"/>
-      <c r="HA3" s="77"/>
-      <c r="HB3" s="78"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="76"/>
+      <c r="R3" s="76"/>
+      <c r="S3" s="76"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="76"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="76"/>
+      <c r="Z3" s="76"/>
+      <c r="AA3" s="76"/>
+      <c r="AB3" s="76"/>
+      <c r="AC3" s="76"/>
+      <c r="AD3" s="76"/>
+      <c r="AE3" s="76"/>
+      <c r="AF3" s="76"/>
+      <c r="AG3" s="76"/>
+      <c r="AH3" s="76"/>
+      <c r="AI3" s="76"/>
+      <c r="AJ3" s="76"/>
+      <c r="AK3" s="76"/>
+      <c r="AL3" s="76"/>
+      <c r="AM3" s="76"/>
+      <c r="AN3" s="76"/>
+      <c r="AO3" s="76"/>
+      <c r="AP3" s="76"/>
+      <c r="AQ3" s="76"/>
+      <c r="AR3" s="76"/>
+      <c r="AS3" s="76"/>
+      <c r="AT3" s="76"/>
+      <c r="AU3" s="76"/>
+      <c r="AV3" s="76"/>
+      <c r="AW3" s="76"/>
+      <c r="AX3" s="76"/>
+      <c r="AY3" s="76"/>
+      <c r="AZ3" s="76"/>
+      <c r="BA3" s="76"/>
+      <c r="BB3" s="76"/>
+      <c r="BC3" s="76"/>
+      <c r="BD3" s="76"/>
+      <c r="BE3" s="76"/>
+      <c r="BF3" s="76"/>
+      <c r="BG3" s="76"/>
+      <c r="BH3" s="76"/>
+      <c r="BI3" s="76"/>
+      <c r="BJ3" s="76"/>
+      <c r="BK3" s="76"/>
+      <c r="BL3" s="76"/>
+      <c r="BM3" s="76"/>
+      <c r="BN3" s="76"/>
+      <c r="BO3" s="76"/>
+      <c r="BP3" s="76"/>
+      <c r="BQ3" s="76"/>
+      <c r="BR3" s="76"/>
+      <c r="BS3" s="76"/>
+      <c r="BT3" s="76"/>
+      <c r="BU3" s="76"/>
+      <c r="BV3" s="76"/>
+      <c r="BW3" s="76"/>
+      <c r="BX3" s="76"/>
+      <c r="BY3" s="76"/>
+      <c r="BZ3" s="76"/>
+      <c r="CA3" s="76"/>
+      <c r="CB3" s="76"/>
+      <c r="CC3" s="76"/>
+      <c r="CD3" s="76"/>
+      <c r="CE3" s="76"/>
+      <c r="CF3" s="76"/>
+      <c r="CG3" s="76"/>
+      <c r="CH3" s="76"/>
+      <c r="CI3" s="76"/>
+      <c r="CJ3" s="76"/>
+      <c r="CK3" s="76"/>
+      <c r="CL3" s="76"/>
+      <c r="CM3" s="76"/>
+      <c r="CN3" s="76"/>
+      <c r="CO3" s="76"/>
+      <c r="CP3" s="76"/>
+      <c r="CQ3" s="76"/>
+      <c r="CR3" s="76"/>
+      <c r="CS3" s="76"/>
+      <c r="CT3" s="76"/>
+      <c r="CU3" s="76"/>
+      <c r="CV3" s="76"/>
+      <c r="CW3" s="76"/>
+      <c r="CX3" s="76"/>
+      <c r="CY3" s="76"/>
+      <c r="CZ3" s="76"/>
+      <c r="DA3" s="76"/>
+      <c r="DB3" s="76"/>
+      <c r="DC3" s="76"/>
+      <c r="DD3" s="76"/>
+      <c r="DE3" s="76"/>
+      <c r="DF3" s="76"/>
+      <c r="DG3" s="76"/>
+      <c r="DH3" s="76"/>
+      <c r="DI3" s="76"/>
+      <c r="DJ3" s="76"/>
+      <c r="DK3" s="76"/>
+      <c r="DL3" s="76"/>
+      <c r="DM3" s="76"/>
+      <c r="DN3" s="76"/>
+      <c r="DO3" s="76"/>
+      <c r="DP3" s="76"/>
+      <c r="DQ3" s="76"/>
+      <c r="DR3" s="76"/>
+      <c r="DS3" s="76"/>
+      <c r="DT3" s="76"/>
+      <c r="DU3" s="76"/>
+      <c r="DV3" s="76"/>
+      <c r="DW3" s="76"/>
+      <c r="DX3" s="76"/>
+      <c r="DY3" s="76"/>
+      <c r="DZ3" s="76"/>
+      <c r="EA3" s="76"/>
+      <c r="EB3" s="76"/>
+      <c r="EC3" s="76"/>
+      <c r="ED3" s="76"/>
+      <c r="EE3" s="76"/>
+      <c r="EF3" s="76"/>
+      <c r="EG3" s="76"/>
+      <c r="EH3" s="76"/>
+      <c r="EI3" s="76"/>
+      <c r="EJ3" s="76"/>
+      <c r="EK3" s="76"/>
+      <c r="EL3" s="76"/>
+      <c r="EM3" s="76"/>
+      <c r="EN3" s="76"/>
+      <c r="EO3" s="76"/>
+      <c r="EP3" s="76"/>
+      <c r="EQ3" s="76"/>
+      <c r="ER3" s="76"/>
+      <c r="ES3" s="76"/>
+      <c r="ET3" s="76"/>
+      <c r="EU3" s="76"/>
+      <c r="EV3" s="76"/>
+      <c r="EW3" s="76"/>
+      <c r="EX3" s="76"/>
+      <c r="EY3" s="76"/>
+      <c r="EZ3" s="76"/>
+      <c r="FA3" s="76"/>
+      <c r="FB3" s="76"/>
+      <c r="FC3" s="76"/>
+      <c r="FD3" s="76"/>
+      <c r="FE3" s="76"/>
+      <c r="FF3" s="76"/>
+      <c r="FG3" s="76"/>
+      <c r="FH3" s="76"/>
+      <c r="FI3" s="76"/>
+      <c r="FJ3" s="76"/>
+      <c r="FK3" s="76"/>
+      <c r="FL3" s="76"/>
+      <c r="FM3" s="76"/>
+      <c r="FN3" s="76"/>
+      <c r="FO3" s="76"/>
+      <c r="FP3" s="76"/>
+      <c r="FQ3" s="76"/>
+      <c r="FR3" s="76"/>
+      <c r="FS3" s="76"/>
+      <c r="FT3" s="76"/>
+      <c r="FU3" s="76"/>
+      <c r="FV3" s="76"/>
+      <c r="FW3" s="76"/>
+      <c r="FX3" s="76"/>
+      <c r="FY3" s="76"/>
+      <c r="FZ3" s="76"/>
+      <c r="GA3" s="76"/>
+      <c r="GB3" s="76"/>
+      <c r="GC3" s="76"/>
+      <c r="GD3" s="76"/>
+      <c r="GE3" s="76"/>
+      <c r="GF3" s="76"/>
+      <c r="GG3" s="76"/>
+      <c r="GH3" s="76"/>
+      <c r="GI3" s="76"/>
+      <c r="GJ3" s="76"/>
+      <c r="GK3" s="76"/>
+      <c r="GL3" s="76"/>
+      <c r="GM3" s="76"/>
+      <c r="GN3" s="76"/>
+      <c r="GO3" s="76"/>
+      <c r="GP3" s="76"/>
+      <c r="GQ3" s="76"/>
+      <c r="GR3" s="76"/>
+      <c r="GS3" s="76"/>
+      <c r="GT3" s="76"/>
+      <c r="GU3" s="76"/>
+      <c r="GV3" s="76"/>
+      <c r="GW3" s="76"/>
+      <c r="GX3" s="76"/>
+      <c r="GY3" s="76"/>
+      <c r="GZ3" s="76"/>
+      <c r="HA3" s="76"/>
+      <c r="HB3" s="77"/>
     </row>
     <row r="4" spans="2:210" x14ac:dyDescent="0.25">
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="85" t="s">
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="87"/>
-      <c r="H4" s="85" t="s">
+      <c r="G4" s="86"/>
+      <c r="H4" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="91"/>
-      <c r="J4" s="87"/>
+      <c r="I4" s="90"/>
+      <c r="J4" s="86"/>
       <c r="K4" s="57" t="s">
         <v>28</v>
       </c>
@@ -2531,16 +2530,16 @@
       <c r="HB4" s="46"/>
     </row>
     <row r="5" spans="2:210" x14ac:dyDescent="0.25">
-      <c r="B5" s="88"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="58" t="s">
+      <c r="B5" s="87"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="92" t="s">
         <v>36</v>
       </c>
       <c r="L5" s="47"/>
@@ -2744,15 +2743,15 @@
       <c r="HB5" s="49"/>
     </row>
     <row r="6" spans="2:210" x14ac:dyDescent="0.25">
-      <c r="B6" s="88"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="90"/>
+      <c r="B6" s="87"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="89"/>
       <c r="K6" s="56" t="s">
         <v>29</v>
       </c>
@@ -2960,10 +2959,10 @@
       <c r="B7" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="59" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="54" t="s">
@@ -2984,7 +2983,7 @@
       <c r="J7" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="59" t="s">
+      <c r="K7" s="58" t="s">
         <v>30</v>
       </c>
       <c r="L7" s="50"/>
@@ -3189,15 +3188,15 @@
     </row>
     <row r="8" spans="2:210" x14ac:dyDescent="0.25">
       <c r="B8" s="32"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="61"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="60"/>
       <c r="E8" s="33"/>
       <c r="F8" s="32"/>
       <c r="G8" s="33"/>
       <c r="H8" s="38"/>
       <c r="I8" s="39"/>
       <c r="J8" s="36"/>
-      <c r="K8" s="81"/>
+      <c r="K8" s="80"/>
       <c r="L8" s="38"/>
       <c r="M8" s="39"/>
       <c r="N8" s="39"/>
@@ -3399,7 +3398,7 @@
       <c r="HB8" s="42"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="b9tuTLARKu+npNCDEFVyX6rLYptCWG/H620wCfRN9N8L0ML0Q6ymY/WjQYtGDERpuOSS4k19djumr1k/VUs4bQ==" saltValue="AgqhqEmU0OP51lXlqtAX1Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="7">
     <mergeCell ref="L3:HB3"/>
     <mergeCell ref="K2:K3"/>
@@ -3420,7 +3419,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:G7 J7 E7 K4 K6:K7 K5" xr:uid="{CE00ACBD-26F6-4D31-8815-799B3F12B44D}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:G7 J7 E7 K4 K6:K7" xr:uid="{CE00ACBD-26F6-4D31-8815-799B3F12B44D}">
       <formula1>"&lt;0&gt;0"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3430,9 +3429,8 @@
     <hyperlink ref="J7" r:id="rId3" location="raisings" xr:uid="{D5998F8A-5538-4B97-A69F-87F4C6FD227B}"/>
     <hyperlink ref="K6" r:id="rId4" location="raisings" xr:uid="{734FEA83-F7F5-4752-9BA7-447F52D8CCBF}"/>
     <hyperlink ref="K4" r:id="rId5" location="allSpecies" xr:uid="{2A2779B2-525B-441C-AE45-EA909D481D6A}"/>
-    <hyperlink ref="K5" r:id="rId6" location="fates" xr:uid="{2AED1A41-AA2C-4021-85BA-4B774F6093E9}"/>
-    <hyperlink ref="K7" r:id="rId7" location="catchUnits" xr:uid="{1D8DEE0F-0F12-40CC-8B2D-769700ED1998}"/>
-    <hyperlink ref="E7" r:id="rId8" location="IOgrids1x1" xr:uid="{49876D03-0E52-4AC4-9B57-EA347F24B506}"/>
+    <hyperlink ref="K7" r:id="rId6" location="catchUnits" xr:uid="{1D8DEE0F-0F12-40CC-8B2D-769700ED1998}"/>
+    <hyperlink ref="E7" r:id="rId7" location="IOgrids1x1" xr:uid="{49876D03-0E52-4AC4-9B57-EA347F24B506}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>